<commit_message>
add check nic's gw
</commit_message>
<xml_diff>
--- a/IP.xlsx
+++ b/IP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programing\C#\setip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB29F5C-1FE2-46C0-BC9D-845617F7E717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1747A2DA-C0E2-47E1-A0BD-CF03054909A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="14400" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>OLD_IP</t>
   </si>
@@ -35,98 +35,6 @@
   </si>
   <si>
     <t>NEW_DNS</t>
-  </si>
-  <si>
-    <t>10.0.0.1</t>
-  </si>
-  <si>
-    <t>255.255.255.0</t>
-  </si>
-  <si>
-    <t>10.0.0.2</t>
-  </si>
-  <si>
-    <t>10.0.0.3</t>
-  </si>
-  <si>
-    <t>10.0.0.4</t>
-  </si>
-  <si>
-    <t>10.0.0.5</t>
-  </si>
-  <si>
-    <t>10.0.0.6</t>
-  </si>
-  <si>
-    <t>10.0.0.7</t>
-  </si>
-  <si>
-    <t>10.0.0.8</t>
-  </si>
-  <si>
-    <t>10.0.0.9</t>
-  </si>
-  <si>
-    <t>10.0.0.10</t>
-  </si>
-  <si>
-    <t>10.0.0.11</t>
-  </si>
-  <si>
-    <t>10.0.0.12</t>
-  </si>
-  <si>
-    <t>10.0.0.13</t>
-  </si>
-  <si>
-    <t>10.0.0.14</t>
-  </si>
-  <si>
-    <t>192.168.255.1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>192.168.255.2</t>
-  </si>
-  <si>
-    <t>192.168.255.3</t>
-  </si>
-  <si>
-    <t>192.168.255.4</t>
-  </si>
-  <si>
-    <t>192.168.255.5</t>
-  </si>
-  <si>
-    <t>192.168.255.6</t>
-  </si>
-  <si>
-    <t>192.168.255.7</t>
-  </si>
-  <si>
-    <t>192.168.255.8</t>
-  </si>
-  <si>
-    <t>192.168.255.9</t>
-  </si>
-  <si>
-    <t>192.168.255.10</t>
-  </si>
-  <si>
-    <t>192.168.255.11</t>
-  </si>
-  <si>
-    <t>192.168.255.12</t>
-  </si>
-  <si>
-    <t>192.168.255.13</t>
-  </si>
-  <si>
-    <t>192.168.255.14</t>
-  </si>
-  <si>
-    <t>180.76.76.76</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -498,7 +406,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E15"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -527,242 +435,102 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>